<commit_message>
added missing folders, parameter values
</commit_message>
<xml_diff>
--- a/VRNN_theano_version/output/vrnn-dis1-dataport.xlsx
+++ b/VRNN_theano_version/output/vrnn-dis1-dataport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all-builds" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="222">
   <si>
     <t xml:space="preserve">epochs</t>
   </si>
@@ -3119,8 +3119,8 @@
   </sheetPr>
   <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N123" activeCellId="0" sqref="N123"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G69" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z126" activeCellId="0" sqref="Z126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7048,6 +7048,24 @@
       <c r="S95" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="T95" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U95" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V95" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W95" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X95" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y95" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z95" s="0" t="s">
         <v>115</v>
       </c>
@@ -7110,6 +7128,24 @@
       <c r="S96" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="T96" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U96" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V96" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W96" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X96" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y96" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z96" s="0" t="s">
         <v>115</v>
       </c>
@@ -7169,6 +7205,27 @@
       <c r="R97" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S97" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T97" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U97" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V97" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W97" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X97" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y97" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z97" s="0" t="s">
         <v>115</v>
       </c>
@@ -7228,6 +7285,27 @@
       <c r="R98" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S98" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T98" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U98" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V98" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W98" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X98" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y98" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z98" s="0" t="s">
         <v>115</v>
       </c>
@@ -7287,6 +7365,27 @@
       <c r="R99" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S99" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T99" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U99" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V99" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W99" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X99" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y99" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z99" s="0" t="s">
         <v>115</v>
       </c>
@@ -7346,6 +7445,27 @@
       <c r="R100" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S100" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T100" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U100" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V100" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W100" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X100" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y100" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z100" s="0" t="s">
         <v>115</v>
       </c>
@@ -7405,6 +7525,27 @@
       <c r="R101" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T101" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U101" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V101" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y101" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z101" s="0" t="s">
         <v>115</v>
       </c>
@@ -7464,6 +7605,27 @@
       <c r="R102" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="S102" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T102" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U102" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V102" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W102" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X102" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y102" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z102" s="0" t="s">
         <v>115</v>
       </c>
@@ -7520,6 +7682,30 @@
       <c r="Q103" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="R103" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S103" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T103" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U103" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V103" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W103" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X103" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y103" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z103" s="0" t="s">
         <v>115</v>
       </c>
@@ -7576,6 +7762,30 @@
       <c r="Q104" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="R104" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S104" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T104" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U104" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V104" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W104" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X104" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y104" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z104" s="0" t="s">
         <v>115</v>
       </c>
@@ -7632,6 +7842,30 @@
       <c r="Q105" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="R105" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T105" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U105" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V105" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y105" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z105" s="0" t="s">
         <v>115</v>
       </c>
@@ -7688,6 +7922,30 @@
       <c r="Q106" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="R106" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S106" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T106" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U106" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V106" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W106" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X106" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y106" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z106" s="0" t="s">
         <v>115</v>
       </c>
@@ -7744,6 +8002,33 @@
       <c r="Q109" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="R109" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S109" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T109" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U109" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V109" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W109" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X109" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y109" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z109" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
@@ -7797,6 +8082,33 @@
       <c r="Q110" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="R110" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S110" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T110" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U110" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V110" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W110" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X110" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y110" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z110" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
@@ -7850,6 +8162,33 @@
       <c r="Q111" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="R111" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S111" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T111" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U111" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V111" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W111" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X111" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y111" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z111" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
@@ -7903,6 +8242,30 @@
       <c r="Q113" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="R113" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S113" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T113" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U113" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V113" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W113" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X113" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y113" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z113" s="0" t="n">
         <v>30</v>
       </c>
@@ -7959,6 +8322,30 @@
       <c r="Q114" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="R114" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S114" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T114" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U114" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V114" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W114" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X114" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y114" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z114" s="0" t="n">
         <v>30</v>
       </c>
@@ -8015,6 +8402,30 @@
       <c r="Q115" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="R115" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S115" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T115" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U115" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V115" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W115" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X115" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y115" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z115" s="0" t="n">
         <v>30</v>
       </c>
@@ -8071,6 +8482,30 @@
       <c r="Q116" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="R116" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S116" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T116" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U116" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V116" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W116" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X116" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y116" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z116" s="0" t="n">
         <v>30</v>
       </c>
@@ -8127,6 +8562,30 @@
       <c r="Q117" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="R117" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S117" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T117" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U117" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V117" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W117" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X117" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y117" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z117" s="0" t="n">
         <v>30</v>
       </c>
@@ -8183,6 +8642,30 @@
       <c r="Q118" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="R118" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S118" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T118" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U118" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V118" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W118" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X118" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y118" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="Z118" s="0" t="n">
         <v>30</v>
       </c>
@@ -8245,6 +8728,27 @@
       <c r="S119" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="T119" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U119" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V119" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W119" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X119" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y119" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z119" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
@@ -8298,6 +8802,33 @@
       <c r="Q120" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="R120" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S120" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T120" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U120" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V120" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W120" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X120" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y120" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z120" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
@@ -8351,6 +8882,33 @@
       <c r="Q121" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="R121" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="S121" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T121" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U121" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V121" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W121" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X121" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y121" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z121" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
@@ -8409,6 +8967,27 @@
       </c>
       <c r="S123" s="0" t="n">
         <v>150</v>
+      </c>
+      <c r="T123" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="U123" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="V123" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W123" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="X123" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y123" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z123" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>